<commit_message>
SQL AND DATA REFIX
</commit_message>
<xml_diff>
--- a/Data/11. 지역.xlsx
+++ b/Data/11. 지역.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\내 드라이브\학교\3학년(4.5)(2023)\2학기\데이터베이스프로그래밍\과제\팀프로젝트\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SUBCOM\Desktop\Gitkraken\DatabaseProgrammingTeamProject\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B86C1E18-A4E4-481C-90CC-F2E36DA45D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7E836C-1138-4B36-A122-847977127A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{9DBD8AB9-FAF1-4A7C-A5AF-D57D4485BB31}"/>
+    <workbookView xWindow="5565" yWindow="1080" windowWidth="28800" windowHeight="15435" xr2:uid="{9DBD8AB9-FAF1-4A7C-A5AF-D57D4485BB31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>지역</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -160,13 +160,58 @@
   <si>
     <t>군산</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>용인</t>
+  </si>
+  <si>
+    <t>화성</t>
+  </si>
+  <si>
+    <t>동두천</t>
+  </si>
+  <si>
+    <t>평택</t>
+  </si>
+  <si>
+    <t>의왕</t>
+  </si>
+  <si>
+    <t>공주</t>
+  </si>
+  <si>
+    <t>경기</t>
+  </si>
+  <si>
+    <t>군포</t>
+  </si>
+  <si>
+    <t>이천</t>
+  </si>
+  <si>
+    <t>안산</t>
+  </si>
+  <si>
+    <t>서천군</t>
+  </si>
+  <si>
+    <t>충북</t>
+  </si>
+  <si>
+    <t>전남</t>
+  </si>
+  <si>
+    <t>전북</t>
+  </si>
+  <si>
+    <t>충남</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,6 +230,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF374151"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -213,12 +266,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -534,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61BBA2F-961A-41DA-887C-332BDA830D18}">
-  <dimension ref="A1:A31"/>
+  <dimension ref="A1:A46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -697,6 +753,81 @@
         <v>30</v>
       </c>
     </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>